<commit_message>
Job Add/Remove modal Contractor modal Work open/close
</commit_message>
<xml_diff>
--- a/TimeCardCore/wwwroot/content/TimeCardTemplates.xlsx
+++ b/TimeCardCore/wwwroot/content/TimeCardTemplates.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Greg\source\repos\TimeCard\TimeCard\Content\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Greg\source\repos\TimeCardCore\TimeCardCore\wwwroot\content\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7BB62D1-2507-4F8C-9384-BA18F624F591}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA0C60BA-EA34-4667-9FF4-81DA60D2201F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3570" yWindow="3270" windowWidth="23760" windowHeight="12615" activeTab="1" xr2:uid="{E5B8759E-483A-4A2C-BBDA-A83D80136576}"/>
+    <workbookView xWindow="3465" yWindow="3465" windowWidth="20910" windowHeight="11835" activeTab="2" xr2:uid="{E5B8759E-483A-4A2C-BBDA-A83D80136576}"/>
   </bookViews>
   <sheets>
     <sheet name="TimeBook" sheetId="3" r:id="rId1"/>
@@ -138,16 +138,9 @@
     <t>INVOICE</t>
   </si>
   <si>
-    <t>Opal Software, LLC</t>
-  </si>
-  <si>
     <t xml:space="preserve">DATE: </t>
   </si>
   <si>
-    <t>824 W. Safari Dr.
-Tucson, AZ  85704</t>
-  </si>
-  <si>
     <t xml:space="preserve"> </t>
   </si>
   <si>
@@ -224,6 +217,12 @@
   </si>
   <si>
     <t>Payment      Details</t>
+  </si>
+  <si>
+    <t>[Contractor Corp.]</t>
+  </si>
+  <si>
+    <t>[Contractor Address]</t>
   </si>
 </sst>
 </file>
@@ -645,7 +644,7 @@
     <xf numFmtId="0" fontId="26" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="27" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="105">
+  <cellXfs count="106">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -748,12 +747,6 @@
     <xf numFmtId="14" fontId="19" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="19" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="19" fillId="0" borderId="0" xfId="9" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
@@ -827,6 +820,24 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="14" fontId="19" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="24" fillId="2" borderId="15" xfId="10" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -872,20 +883,11 @@
     <xf numFmtId="14" fontId="11" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment vertical="top"/>
+    <xf numFmtId="2" fontId="19" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="19" fillId="0" borderId="0" xfId="9" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="14">
@@ -1385,23 +1387,23 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.28515625" customWidth="1"/>
-    <col min="3" max="3" width="9.140625" style="65"/>
+    <col min="3" max="3" width="9.140625" style="63"/>
     <col min="4" max="4" width="105.42578125" customWidth="1"/>
     <col min="5" max="5" width="15.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="78" t="s">
-        <v>43</v>
-      </c>
-      <c r="B1" s="79" t="s">
-        <v>44</v>
-      </c>
-      <c r="C1" s="80" t="s">
-        <v>49</v>
-      </c>
-      <c r="D1" s="81" t="s">
+      <c r="A1" s="76" t="s">
+        <v>41</v>
+      </c>
+      <c r="B1" s="77" t="s">
+        <v>42</v>
+      </c>
+      <c r="C1" s="78" t="s">
         <v>47</v>
+      </c>
+      <c r="D1" s="79" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
@@ -1414,16 +1416,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00EC0102-26B9-496D-8FD1-279AC5F04544}">
   <dimension ref="A1:K8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A7" sqref="A7:K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.140625" style="68" customWidth="1"/>
+    <col min="1" max="1" width="25.140625" style="66" customWidth="1"/>
     <col min="2" max="2" width="14.5703125" customWidth="1"/>
-    <col min="3" max="3" width="9.85546875" style="66" customWidth="1"/>
-    <col min="4" max="4" width="10.42578125" style="66" customWidth="1"/>
+    <col min="3" max="3" width="9.85546875" style="64" customWidth="1"/>
+    <col min="4" max="4" width="10.42578125" style="64" customWidth="1"/>
     <col min="5" max="5" width="10.7109375" customWidth="1"/>
     <col min="6" max="6" width="10.42578125" customWidth="1"/>
     <col min="7" max="8" width="13.28515625" customWidth="1"/>
@@ -1433,103 +1435,103 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="69" t="s">
+      <c r="A1" s="67" t="s">
+        <v>48</v>
+      </c>
+      <c r="B1" s="68" t="s">
+        <v>49</v>
+      </c>
+      <c r="C1" s="69" t="s">
+        <v>42</v>
+      </c>
+      <c r="D1" s="69" t="s">
         <v>50</v>
       </c>
-      <c r="B1" s="70" t="s">
+    </row>
+    <row r="2" spans="1:11" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="65"/>
+      <c r="B2" s="80"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="65"/>
+      <c r="B3" s="80"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="65"/>
+    </row>
+    <row r="5" spans="1:11" s="73" customFormat="1" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="70"/>
+      <c r="B5" s="71"/>
+      <c r="C5" s="72"/>
+      <c r="D5" s="72"/>
+      <c r="E5" s="71"/>
+      <c r="F5" s="71"/>
+      <c r="G5" s="71"/>
+      <c r="H5" s="71"/>
+      <c r="I5" s="87" t="s">
+        <v>60</v>
+      </c>
+      <c r="J5" s="87"/>
+      <c r="K5" s="87"/>
+    </row>
+    <row r="6" spans="1:11" s="73" customFormat="1" ht="18.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="67" t="s">
         <v>51</v>
       </c>
-      <c r="C1" s="71" t="s">
-        <v>44</v>
-      </c>
-      <c r="D1" s="71" t="s">
+      <c r="B6" s="68" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6" s="74" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="67"/>
-      <c r="B2" s="82"/>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="67"/>
-      <c r="B3" s="82"/>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="67"/>
-    </row>
-    <row r="5" spans="1:11" s="75" customFormat="1" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="72"/>
-      <c r="B5" s="73"/>
-      <c r="C5" s="74"/>
-      <c r="D5" s="74"/>
-      <c r="E5" s="73"/>
-      <c r="F5" s="73"/>
-      <c r="G5" s="73"/>
-      <c r="H5" s="73"/>
-      <c r="I5" s="83" t="s">
-        <v>62</v>
-      </c>
-      <c r="J5" s="83"/>
-      <c r="K5" s="83"/>
-    </row>
-    <row r="6" spans="1:11" s="75" customFormat="1" ht="18.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="69" t="s">
+      <c r="D6" s="69" t="s">
+        <v>59</v>
+      </c>
+      <c r="E6" s="69" t="s">
         <v>53</v>
       </c>
-      <c r="B6" s="70" t="s">
-        <v>24</v>
-      </c>
-      <c r="C6" s="76" t="s">
+      <c r="F6" s="75" t="s">
         <v>54</v>
       </c>
-      <c r="D6" s="71" t="s">
-        <v>61</v>
-      </c>
-      <c r="E6" s="71" t="s">
+      <c r="G6" s="75" t="s">
         <v>55</v>
       </c>
-      <c r="F6" s="77" t="s">
+      <c r="H6" s="75" t="s">
         <v>56</v>
       </c>
-      <c r="G6" s="77" t="s">
+      <c r="I6" s="75" t="s">
+        <v>42</v>
+      </c>
+      <c r="J6" s="75" t="s">
         <v>57</v>
       </c>
-      <c r="H6" s="77" t="s">
+      <c r="K6" s="75" t="s">
         <v>58</v>
       </c>
-      <c r="I6" s="77" t="s">
-        <v>44</v>
-      </c>
-      <c r="J6" s="77" t="s">
-        <v>59</v>
-      </c>
-      <c r="K6" s="77" t="s">
-        <v>60</v>
-      </c>
     </row>
     <row r="7" spans="1:11" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="68"/>
-      <c r="C7" s="100"/>
-      <c r="D7" s="101"/>
-      <c r="E7" s="101"/>
-      <c r="F7" s="101"/>
-      <c r="G7" s="102"/>
-      <c r="H7" s="103"/>
-      <c r="I7" s="101"/>
-      <c r="J7" s="103"/>
-      <c r="K7" s="102"/>
+      <c r="B7" s="66"/>
+      <c r="C7" s="81"/>
+      <c r="D7" s="82"/>
+      <c r="E7" s="82"/>
+      <c r="F7" s="82"/>
+      <c r="G7" s="83"/>
+      <c r="H7" s="84"/>
+      <c r="I7" s="82"/>
+      <c r="J7" s="84"/>
+      <c r="K7" s="83"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B8" s="68"/>
-      <c r="C8" s="100"/>
-      <c r="D8" s="101"/>
-      <c r="E8" s="104"/>
-      <c r="F8" s="104"/>
-      <c r="G8" s="102"/>
-      <c r="H8" s="103"/>
-      <c r="I8" s="104"/>
-      <c r="J8" s="103"/>
-      <c r="K8" s="102"/>
+      <c r="B8" s="66"/>
+      <c r="C8" s="81"/>
+      <c r="D8" s="82"/>
+      <c r="E8" s="85"/>
+      <c r="F8" s="85"/>
+      <c r="G8" s="83"/>
+      <c r="H8" s="84"/>
+      <c r="I8" s="85"/>
+      <c r="J8" s="84"/>
+      <c r="K8" s="83"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1548,8 +1550,8 @@
   </sheetPr>
   <dimension ref="A1:F17"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11:XFD11"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1564,20 +1566,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="42.95" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B1" s="85" t="s">
+      <c r="B1" s="89" t="s">
         <v>33</v>
       </c>
-      <c r="C1" s="85"/>
-      <c r="D1" s="85"/>
-      <c r="E1" s="85"/>
+      <c r="C1" s="89"/>
+      <c r="D1" s="89"/>
+      <c r="E1" s="89"/>
     </row>
     <row r="2" spans="1:6" ht="36.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B2" s="46" t="s">
-        <v>34</v>
+        <v>61</v>
       </c>
       <c r="C2" s="46"/>
       <c r="D2" s="47" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E2" s="47"/>
       <c r="F2" s="48">
@@ -1585,43 +1587,43 @@
       </c>
     </row>
     <row r="3" spans="1:6" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="86" t="s">
-        <v>36</v>
-      </c>
-      <c r="C3" s="86"/>
+      <c r="B3" s="90" t="s">
+        <v>62</v>
+      </c>
+      <c r="C3" s="90"/>
       <c r="D3" s="47"/>
       <c r="E3" s="47"/>
       <c r="F3" s="45" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="49" t="s">
+        <v>36</v>
+      </c>
+      <c r="C4" s="49"/>
+      <c r="D4" s="91" t="s">
+        <v>35</v>
+      </c>
+      <c r="E4" s="91"/>
+    </row>
+    <row r="5" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="92" t="s">
+        <v>37</v>
+      </c>
+      <c r="C5" s="92"/>
+    </row>
+    <row r="6" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="90" t="s">
         <v>38</v>
       </c>
-      <c r="C4" s="49"/>
-      <c r="D4" s="87" t="s">
-        <v>37</v>
-      </c>
-      <c r="E4" s="87"/>
-    </row>
-    <row r="5" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="88" t="s">
-        <v>39</v>
-      </c>
-      <c r="C5" s="88"/>
-    </row>
-    <row r="6" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="86" t="s">
-        <v>40</v>
-      </c>
-      <c r="C6" s="86"/>
+      <c r="C6" s="90"/>
     </row>
     <row r="7" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="86" t="s">
+      <c r="B7" s="90" t="s">
         <v>2</v>
       </c>
-      <c r="C7" s="86"/>
+      <c r="C7" s="90"/>
     </row>
     <row r="8" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="50"/>
@@ -1630,82 +1632,82 @@
     <row r="9" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="51"/>
       <c r="B9" s="49" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C9" s="50"/>
     </row>
     <row r="10" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="51"/>
       <c r="B10" s="52" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C10" s="52"/>
     </row>
-    <row r="11" spans="1:6" s="54" customFormat="1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" s="54" customFormat="1" ht="11.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="51"/>
       <c r="B11" s="52" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C11" s="52">
-        <v>52</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="51"/>
       <c r="B12" s="53" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C12" s="53"/>
     </row>
     <row r="13" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="51"/>
-      <c r="B13" s="59" t="s">
+      <c r="B13" s="57" t="s">
+        <v>41</v>
+      </c>
+      <c r="C13" s="57" t="s">
+        <v>22</v>
+      </c>
+      <c r="D13" s="58" t="s">
+        <v>42</v>
+      </c>
+      <c r="E13" s="57" t="s">
+        <v>35</v>
+      </c>
+      <c r="F13" s="59" t="s">
         <v>43</v>
       </c>
-      <c r="C13" s="59" t="s">
-        <v>22</v>
-      </c>
-      <c r="D13" s="60" t="s">
+    </row>
+    <row r="14" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B14" s="86" t="s">
+        <v>35</v>
+      </c>
+      <c r="C14" s="55"/>
+      <c r="D14" s="104"/>
+      <c r="E14" s="56"/>
+      <c r="F14" s="105"/>
+    </row>
+    <row r="15" spans="1:6" ht="24" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="60" t="s">
         <v>44</v>
       </c>
-      <c r="E13" s="59" t="s">
-        <v>37</v>
-      </c>
-      <c r="F13" s="61" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="55" t="s">
-        <v>37</v>
-      </c>
-      <c r="C14" s="55"/>
-      <c r="D14" s="56"/>
-      <c r="E14" s="58"/>
-      <c r="F14" s="57"/>
-    </row>
-    <row r="15" spans="1:6" ht="24" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="62" t="s">
-        <v>46</v>
-      </c>
-      <c r="C15" s="62"/>
-      <c r="D15" s="63"/>
-      <c r="E15" s="62"/>
-      <c r="F15" s="64"/>
+      <c r="C15" s="60"/>
+      <c r="D15" s="61"/>
+      <c r="E15" s="60"/>
+      <c r="F15" s="62"/>
     </row>
     <row r="16" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="84" t="s">
-        <v>37</v>
-      </c>
-      <c r="C16" s="84"/>
-      <c r="D16" s="84"/>
+      <c r="B16" s="88" t="s">
+        <v>35</v>
+      </c>
+      <c r="C16" s="88"/>
+      <c r="D16" s="88"/>
     </row>
     <row r="17" spans="2:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="84" t="s">
-        <v>37</v>
-      </c>
-      <c r="C17" s="84"/>
-      <c r="D17" s="84"/>
+      <c r="B17" s="88" t="s">
+        <v>35</v>
+      </c>
+      <c r="C17" s="88"/>
+      <c r="D17" s="88"/>
     </row>
   </sheetData>
   <mergeCells count="8">
@@ -1778,37 +1780,37 @@
   <sheetData>
     <row r="1" spans="1:27" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A1" s="1"/>
-      <c r="K1" s="94" t="s">
+      <c r="K1" s="98" t="s">
         <v>0</v>
       </c>
-      <c r="L1" s="95"/>
-      <c r="M1" s="95"/>
+      <c r="L1" s="99"/>
+      <c r="M1" s="99"/>
     </row>
     <row r="2" spans="1:27" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G2" s="3"/>
       <c r="I2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="K2" s="95"/>
-      <c r="L2" s="95"/>
-      <c r="M2" s="95"/>
+      <c r="K2" s="99"/>
+      <c r="L2" s="99"/>
+      <c r="M2" s="99"/>
     </row>
     <row r="3" spans="1:27" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G3" s="5"/>
       <c r="I3" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="K3" s="95"/>
-      <c r="L3" s="95"/>
-      <c r="M3" s="95"/>
+      <c r="K3" s="99"/>
+      <c r="L3" s="99"/>
+      <c r="M3" s="99"/>
     </row>
     <row r="4" spans="1:27" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I4" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="K4" s="95"/>
-      <c r="L4" s="95"/>
-      <c r="M4" s="95"/>
+      <c r="K4" s="99"/>
+      <c r="L4" s="99"/>
+      <c r="M4" s="99"/>
     </row>
     <row r="5" spans="1:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="6" spans="1:27" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -1818,18 +1820,18 @@
       <c r="B6" s="8"/>
       <c r="C6" s="8"/>
       <c r="D6" s="9"/>
-      <c r="E6" s="96" t="s">
+      <c r="E6" s="100" t="s">
         <v>5</v>
       </c>
-      <c r="F6" s="90"/>
-      <c r="G6" s="96" t="s">
+      <c r="F6" s="94"/>
+      <c r="G6" s="100" t="s">
         <v>6</v>
       </c>
-      <c r="H6" s="90"/>
-      <c r="I6" s="96" t="s">
+      <c r="H6" s="94"/>
+      <c r="I6" s="100" t="s">
         <v>7</v>
       </c>
-      <c r="J6" s="90"/>
+      <c r="J6" s="94"/>
       <c r="K6" s="10"/>
       <c r="L6" s="11" t="s">
         <v>8</v>
@@ -1857,18 +1859,18 @@
       <c r="B7" s="15"/>
       <c r="C7" s="15"/>
       <c r="D7" s="16"/>
-      <c r="E7" s="97" t="s">
+      <c r="E7" s="101" t="s">
         <v>10</v>
       </c>
-      <c r="F7" s="92"/>
-      <c r="G7" s="98" t="s">
+      <c r="F7" s="96"/>
+      <c r="G7" s="102" t="s">
         <v>11</v>
       </c>
-      <c r="H7" s="92"/>
-      <c r="I7" s="99">
+      <c r="H7" s="96"/>
+      <c r="I7" s="103">
         <v>43455</v>
       </c>
-      <c r="J7" s="92"/>
+      <c r="J7" s="96"/>
       <c r="K7" s="17"/>
       <c r="L7" s="18" t="s">
         <v>12</v>
@@ -1879,10 +1881,10 @@
       <c r="A8" s="20"/>
     </row>
     <row r="9" spans="1:27" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="89" t="s">
+      <c r="A9" s="93" t="s">
         <v>13</v>
       </c>
-      <c r="B9" s="90"/>
+      <c r="B9" s="94"/>
       <c r="C9" s="21"/>
       <c r="D9" s="22"/>
       <c r="E9" s="23" t="s">
@@ -1906,10 +1908,10 @@
       <c r="K9" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="L9" s="91" t="s">
+      <c r="L9" s="95" t="s">
         <v>21</v>
       </c>
-      <c r="M9" s="92"/>
+      <c r="M9" s="96"/>
     </row>
     <row r="10" spans="1:27" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="24" t="s">
@@ -1973,10 +1975,10 @@
       <c r="M11" s="32"/>
     </row>
     <row r="12" spans="1:27" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="93" t="s">
+      <c r="A12" s="97" t="s">
         <v>27</v>
       </c>
-      <c r="B12" s="92"/>
+      <c r="B12" s="96"/>
       <c r="C12" s="30"/>
       <c r="D12" s="33"/>
       <c r="E12" s="32">

</xml_diff>

<commit_message>
Combine Sessions Allow 4 week timecards
</commit_message>
<xml_diff>
--- a/TimeCardCore/wwwroot/content/TimeCardTemplates.xlsx
+++ b/TimeCardCore/wwwroot/content/TimeCardTemplates.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Greg\source\repos\TimeCardCore\TimeCardCore\wwwroot\content\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA0C60BA-EA34-4667-9FF4-81DA60D2201F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40D13100-0188-473C-96A3-67F54692E33B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3465" yWindow="3465" windowWidth="20910" windowHeight="11835" activeTab="2" xr2:uid="{E5B8759E-483A-4A2C-BBDA-A83D80136576}"/>
+    <workbookView xWindow="29610" yWindow="-120" windowWidth="28110" windowHeight="16440" xr2:uid="{E5B8759E-483A-4A2C-BBDA-A83D80136576}"/>
   </bookViews>
   <sheets>
     <sheet name="TimeBook" sheetId="3" r:id="rId1"/>
@@ -23,18 +23,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="63">
   <si>
     <t>TIME CARD</t>
   </si>
@@ -838,6 +832,12 @@
     <xf numFmtId="14" fontId="19" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="2" fontId="19" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="19" fillId="0" borderId="0" xfId="9" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" indent="1"/>
+    </xf>
     <xf numFmtId="0" fontId="24" fillId="2" borderId="15" xfId="10" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -882,12 +882,6 @@
     </xf>
     <xf numFmtId="14" fontId="11" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="19" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="19" fillId="0" borderId="0" xfId="9" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="14">
@@ -1378,21 +1372,22 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{103216F5-7ECA-4628-B2CE-3F61FF9A5992}">
   <sheetPr codeName="Sheet9"/>
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.28515625" customWidth="1"/>
     <col min="3" max="3" width="9.140625" style="63"/>
-    <col min="4" max="4" width="105.42578125" customWidth="1"/>
-    <col min="5" max="5" width="15.5703125" customWidth="1"/>
+    <col min="4" max="4" width="20" style="63" customWidth="1"/>
+    <col min="5" max="5" width="105.42578125" customWidth="1"/>
+    <col min="6" max="6" width="15.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="76" t="s">
         <v>41</v>
       </c>
@@ -1402,11 +1397,14 @@
       <c r="C1" s="78" t="s">
         <v>47</v>
       </c>
-      <c r="D1" s="79" t="s">
+      <c r="D1" s="78" t="s">
+        <v>24</v>
+      </c>
+      <c r="E1" s="79" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1468,11 +1466,11 @@
       <c r="F5" s="71"/>
       <c r="G5" s="71"/>
       <c r="H5" s="71"/>
-      <c r="I5" s="87" t="s">
+      <c r="I5" s="89" t="s">
         <v>60</v>
       </c>
-      <c r="J5" s="87"/>
-      <c r="K5" s="87"/>
+      <c r="J5" s="89"/>
+      <c r="K5" s="89"/>
     </row>
     <row r="6" spans="1:11" s="73" customFormat="1" ht="18.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="67" t="s">
@@ -1550,7 +1548,7 @@
   </sheetPr>
   <dimension ref="A1:F17"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
@@ -1566,12 +1564,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="42.95" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B1" s="89" t="s">
+      <c r="B1" s="91" t="s">
         <v>33</v>
       </c>
-      <c r="C1" s="89"/>
-      <c r="D1" s="89"/>
-      <c r="E1" s="89"/>
+      <c r="C1" s="91"/>
+      <c r="D1" s="91"/>
+      <c r="E1" s="91"/>
     </row>
     <row r="2" spans="1:6" ht="36.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B2" s="46" t="s">
@@ -1587,10 +1585,10 @@
       </c>
     </row>
     <row r="3" spans="1:6" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="90" t="s">
+      <c r="B3" s="92" t="s">
         <v>62</v>
       </c>
-      <c r="C3" s="90"/>
+      <c r="C3" s="92"/>
       <c r="D3" s="47"/>
       <c r="E3" s="47"/>
       <c r="F3" s="45" t="s">
@@ -1602,28 +1600,28 @@
         <v>36</v>
       </c>
       <c r="C4" s="49"/>
-      <c r="D4" s="91" t="s">
+      <c r="D4" s="93" t="s">
         <v>35</v>
       </c>
-      <c r="E4" s="91"/>
+      <c r="E4" s="93"/>
     </row>
     <row r="5" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="92" t="s">
+      <c r="B5" s="94" t="s">
         <v>37</v>
       </c>
-      <c r="C5" s="92"/>
+      <c r="C5" s="94"/>
     </row>
     <row r="6" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="90" t="s">
+      <c r="B6" s="92" t="s">
         <v>38</v>
       </c>
-      <c r="C6" s="90"/>
+      <c r="C6" s="92"/>
     </row>
     <row r="7" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="90" t="s">
+      <c r="B7" s="92" t="s">
         <v>2</v>
       </c>
-      <c r="C7" s="90"/>
+      <c r="C7" s="92"/>
     </row>
     <row r="8" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="50"/>
@@ -1682,9 +1680,9 @@
         <v>35</v>
       </c>
       <c r="C14" s="55"/>
-      <c r="D14" s="104"/>
+      <c r="D14" s="87"/>
       <c r="E14" s="56"/>
-      <c r="F14" s="105"/>
+      <c r="F14" s="88"/>
     </row>
     <row r="15" spans="1:6" ht="24" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B15" s="60" t="s">
@@ -1696,18 +1694,18 @@
       <c r="F15" s="62"/>
     </row>
     <row r="16" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="88" t="s">
+      <c r="B16" s="90" t="s">
         <v>35</v>
       </c>
-      <c r="C16" s="88"/>
-      <c r="D16" s="88"/>
+      <c r="C16" s="90"/>
+      <c r="D16" s="90"/>
     </row>
     <row r="17" spans="2:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="88" t="s">
+      <c r="B17" s="90" t="s">
         <v>35</v>
       </c>
-      <c r="C17" s="88"/>
-      <c r="D17" s="88"/>
+      <c r="C17" s="90"/>
+      <c r="D17" s="90"/>
     </row>
   </sheetData>
   <mergeCells count="8">
@@ -1780,37 +1778,37 @@
   <sheetData>
     <row r="1" spans="1:27" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A1" s="1"/>
-      <c r="K1" s="98" t="s">
+      <c r="K1" s="100" t="s">
         <v>0</v>
       </c>
-      <c r="L1" s="99"/>
-      <c r="M1" s="99"/>
+      <c r="L1" s="101"/>
+      <c r="M1" s="101"/>
     </row>
     <row r="2" spans="1:27" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G2" s="3"/>
       <c r="I2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="K2" s="99"/>
-      <c r="L2" s="99"/>
-      <c r="M2" s="99"/>
+      <c r="K2" s="101"/>
+      <c r="L2" s="101"/>
+      <c r="M2" s="101"/>
     </row>
     <row r="3" spans="1:27" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G3" s="5"/>
       <c r="I3" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="K3" s="99"/>
-      <c r="L3" s="99"/>
-      <c r="M3" s="99"/>
+      <c r="K3" s="101"/>
+      <c r="L3" s="101"/>
+      <c r="M3" s="101"/>
     </row>
     <row r="4" spans="1:27" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I4" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="K4" s="99"/>
-      <c r="L4" s="99"/>
-      <c r="M4" s="99"/>
+      <c r="K4" s="101"/>
+      <c r="L4" s="101"/>
+      <c r="M4" s="101"/>
     </row>
     <row r="5" spans="1:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="6" spans="1:27" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -1820,18 +1818,18 @@
       <c r="B6" s="8"/>
       <c r="C6" s="8"/>
       <c r="D6" s="9"/>
-      <c r="E6" s="100" t="s">
+      <c r="E6" s="102" t="s">
         <v>5</v>
       </c>
-      <c r="F6" s="94"/>
-      <c r="G6" s="100" t="s">
+      <c r="F6" s="96"/>
+      <c r="G6" s="102" t="s">
         <v>6</v>
       </c>
-      <c r="H6" s="94"/>
-      <c r="I6" s="100" t="s">
+      <c r="H6" s="96"/>
+      <c r="I6" s="102" t="s">
         <v>7</v>
       </c>
-      <c r="J6" s="94"/>
+      <c r="J6" s="96"/>
       <c r="K6" s="10"/>
       <c r="L6" s="11" t="s">
         <v>8</v>
@@ -1859,18 +1857,18 @@
       <c r="B7" s="15"/>
       <c r="C7" s="15"/>
       <c r="D7" s="16"/>
-      <c r="E7" s="101" t="s">
+      <c r="E7" s="103" t="s">
         <v>10</v>
       </c>
-      <c r="F7" s="96"/>
-      <c r="G7" s="102" t="s">
+      <c r="F7" s="98"/>
+      <c r="G7" s="104" t="s">
         <v>11</v>
       </c>
-      <c r="H7" s="96"/>
-      <c r="I7" s="103">
+      <c r="H7" s="98"/>
+      <c r="I7" s="105">
         <v>43455</v>
       </c>
-      <c r="J7" s="96"/>
+      <c r="J7" s="98"/>
       <c r="K7" s="17"/>
       <c r="L7" s="18" t="s">
         <v>12</v>
@@ -1881,10 +1879,10 @@
       <c r="A8" s="20"/>
     </row>
     <row r="9" spans="1:27" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="93" t="s">
+      <c r="A9" s="95" t="s">
         <v>13</v>
       </c>
-      <c r="B9" s="94"/>
+      <c r="B9" s="96"/>
       <c r="C9" s="21"/>
       <c r="D9" s="22"/>
       <c r="E9" s="23" t="s">
@@ -1908,10 +1906,10 @@
       <c r="K9" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="L9" s="95" t="s">
+      <c r="L9" s="97" t="s">
         <v>21</v>
       </c>
-      <c r="M9" s="96"/>
+      <c r="M9" s="98"/>
     </row>
     <row r="10" spans="1:27" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="24" t="s">
@@ -1975,10 +1973,10 @@
       <c r="M11" s="32"/>
     </row>
     <row r="12" spans="1:27" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="97" t="s">
+      <c r="A12" s="99" t="s">
         <v>27</v>
       </c>
-      <c r="B12" s="96"/>
+      <c r="B12" s="98"/>
       <c r="C12" s="30"/>
       <c r="D12" s="33"/>
       <c r="E12" s="32">

</xml_diff>

<commit_message>
New 2g TC template
</commit_message>
<xml_diff>
--- a/TimeCardCore/wwwroot/content/TimeCardTemplates.xlsx
+++ b/TimeCardCore/wwwroot/content/TimeCardTemplates.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gcorr\development\TimeCardCore\TimeCardCore\wwwroot\content\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9061A4C-9A8E-4B3F-9F20-0B32E492919C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D178ECB-3E5E-4C6F-91DD-2EB87ABEB436}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2685" yWindow="2685" windowWidth="21600" windowHeight="11385" xr2:uid="{E5B8759E-483A-4A2C-BBDA-A83D80136576}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E5B8759E-483A-4A2C-BBDA-A83D80136576}"/>
   </bookViews>
   <sheets>
     <sheet name="TimeBook" sheetId="3" r:id="rId1"/>
@@ -643,7 +643,7 @@
     <xf numFmtId="0" fontId="26" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="27" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="111">
+  <cellXfs count="110">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -740,31 +740,25 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="8" applyFont="1">
       <alignment horizontal="left" indent="6"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="2">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="13" xfId="7" applyBorder="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="13" xfId="7" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="13" xfId="5" applyBorder="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="14" xfId="2" applyBorder="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="19" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="19" fillId="0" borderId="14" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="13" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="13" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="13" xfId="5" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="14" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="19" fillId="0" borderId="14" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="19" fillId="0" borderId="14" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="19" fillId="0" borderId="14" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -826,32 +820,24 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="14" fontId="19" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="19" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="19" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="19" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="19" fillId="0" borderId="0" xfId="9" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="19" fillId="0" borderId="0" xfId="9" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" indent="1"/>
     </xf>
     <xf numFmtId="14" fontId="24" fillId="2" borderId="15" xfId="10" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="24" fillId="2" borderId="15" xfId="10" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="24" fillId="2" borderId="15" xfId="10" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -897,6 +883,21 @@
     </xf>
     <xf numFmtId="14" fontId="11" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="14">
@@ -1390,38 +1391,39 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.28515625" style="88" customWidth="1"/>
-    <col min="2" max="2" width="9.140625" style="88"/>
-    <col min="3" max="3" width="9.140625" style="63"/>
-    <col min="4" max="4" width="19.7109375" style="91" customWidth="1"/>
+    <col min="1" max="1" width="13.28515625" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" style="61"/>
+    <col min="4" max="4" width="19.7109375" style="87" customWidth="1"/>
     <col min="5" max="5" width="45.5703125" customWidth="1"/>
     <col min="6" max="6" width="15.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="87" t="s">
+      <c r="A1" s="85" t="s">
         <v>41</v>
       </c>
-      <c r="B1" s="89" t="s">
+      <c r="B1" s="86" t="s">
         <v>42</v>
       </c>
-      <c r="C1" s="76" t="s">
+      <c r="C1" s="74" t="s">
         <v>46</v>
       </c>
-      <c r="D1" s="76" t="s">
+      <c r="D1" s="74" t="s">
         <v>24</v>
       </c>
-      <c r="E1" s="77"/>
-    </row>
-    <row r="2" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="92"/>
-      <c r="B2" s="93"/>
-      <c r="E2" s="90"/>
+      <c r="E1" s="75"/>
+    </row>
+    <row r="2" spans="1:5" s="64" customFormat="1" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="105"/>
+      <c r="B2" s="106"/>
+      <c r="C2" s="107"/>
+      <c r="D2" s="108"/>
+      <c r="E2" s="109"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1439,10 +1441,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.140625" style="66" customWidth="1"/>
+    <col min="1" max="1" width="25.140625" style="64" customWidth="1"/>
     <col min="2" max="2" width="14.5703125" customWidth="1"/>
-    <col min="3" max="3" width="9.85546875" style="64" customWidth="1"/>
-    <col min="4" max="4" width="10.42578125" style="64" customWidth="1"/>
+    <col min="3" max="3" width="9.85546875" style="62" customWidth="1"/>
+    <col min="4" max="4" width="10.42578125" style="62" customWidth="1"/>
     <col min="5" max="5" width="10.7109375" customWidth="1"/>
     <col min="6" max="6" width="10.42578125" customWidth="1"/>
     <col min="7" max="8" width="13.28515625" customWidth="1"/>
@@ -1452,103 +1454,103 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="67" t="s">
+      <c r="A1" s="65" t="s">
         <v>47</v>
       </c>
-      <c r="B1" s="68" t="s">
+      <c r="B1" s="66" t="s">
         <v>48</v>
       </c>
-      <c r="C1" s="69" t="s">
+      <c r="C1" s="67" t="s">
         <v>42</v>
       </c>
-      <c r="D1" s="69" t="s">
+      <c r="D1" s="67" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="65"/>
-      <c r="B2" s="78"/>
+      <c r="A2" s="63"/>
+      <c r="B2" s="76"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="65"/>
-      <c r="B3" s="78"/>
+      <c r="A3" s="63"/>
+      <c r="B3" s="76"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="65"/>
-    </row>
-    <row r="5" spans="1:11" s="73" customFormat="1" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="70"/>
-      <c r="B5" s="71"/>
-      <c r="C5" s="72"/>
-      <c r="D5" s="72"/>
-      <c r="E5" s="71"/>
-      <c r="F5" s="71"/>
-      <c r="G5" s="71"/>
-      <c r="H5" s="71"/>
-      <c r="I5" s="94" t="s">
+      <c r="A4" s="63"/>
+    </row>
+    <row r="5" spans="1:11" s="71" customFormat="1" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="68"/>
+      <c r="B5" s="69"/>
+      <c r="C5" s="70"/>
+      <c r="D5" s="70"/>
+      <c r="E5" s="69"/>
+      <c r="F5" s="69"/>
+      <c r="G5" s="69"/>
+      <c r="H5" s="69"/>
+      <c r="I5" s="88" t="s">
         <v>59</v>
       </c>
-      <c r="J5" s="94"/>
-      <c r="K5" s="94"/>
-    </row>
-    <row r="6" spans="1:11" s="73" customFormat="1" ht="18.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="67" t="s">
+      <c r="J5" s="88"/>
+      <c r="K5" s="88"/>
+    </row>
+    <row r="6" spans="1:11" s="71" customFormat="1" ht="18.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="65" t="s">
         <v>50</v>
       </c>
-      <c r="B6" s="68" t="s">
+      <c r="B6" s="66" t="s">
         <v>24</v>
       </c>
-      <c r="C6" s="74" t="s">
+      <c r="C6" s="72" t="s">
         <v>51</v>
       </c>
-      <c r="D6" s="69" t="s">
+      <c r="D6" s="67" t="s">
         <v>58</v>
       </c>
-      <c r="E6" s="69" t="s">
+      <c r="E6" s="67" t="s">
         <v>52</v>
       </c>
-      <c r="F6" s="75" t="s">
+      <c r="F6" s="73" t="s">
         <v>53</v>
       </c>
-      <c r="G6" s="75" t="s">
+      <c r="G6" s="73" t="s">
         <v>54</v>
       </c>
-      <c r="H6" s="75" t="s">
+      <c r="H6" s="73" t="s">
         <v>55</v>
       </c>
-      <c r="I6" s="75" t="s">
+      <c r="I6" s="73" t="s">
         <v>42</v>
       </c>
-      <c r="J6" s="75" t="s">
+      <c r="J6" s="73" t="s">
         <v>56</v>
       </c>
-      <c r="K6" s="75" t="s">
+      <c r="K6" s="73" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="66"/>
-      <c r="C7" s="79"/>
-      <c r="D7" s="80"/>
-      <c r="E7" s="80"/>
-      <c r="F7" s="80"/>
-      <c r="G7" s="81"/>
-      <c r="H7" s="82"/>
-      <c r="I7" s="80"/>
-      <c r="J7" s="82"/>
-      <c r="K7" s="81"/>
+      <c r="B7" s="64"/>
+      <c r="C7" s="77"/>
+      <c r="D7" s="78"/>
+      <c r="E7" s="78"/>
+      <c r="F7" s="78"/>
+      <c r="G7" s="79"/>
+      <c r="H7" s="80"/>
+      <c r="I7" s="78"/>
+      <c r="J7" s="80"/>
+      <c r="K7" s="79"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B8" s="66"/>
-      <c r="C8" s="79"/>
-      <c r="D8" s="80"/>
-      <c r="E8" s="83"/>
-      <c r="F8" s="83"/>
-      <c r="G8" s="81"/>
-      <c r="H8" s="82"/>
-      <c r="I8" s="83"/>
-      <c r="J8" s="82"/>
-      <c r="K8" s="81"/>
+      <c r="B8" s="64"/>
+      <c r="C8" s="77"/>
+      <c r="D8" s="78"/>
+      <c r="E8" s="81"/>
+      <c r="F8" s="81"/>
+      <c r="G8" s="79"/>
+      <c r="H8" s="80"/>
+      <c r="I8" s="81"/>
+      <c r="J8" s="80"/>
+      <c r="K8" s="79"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1583,12 +1585,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="42.95" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B1" s="96" t="s">
+      <c r="B1" s="90" t="s">
         <v>33</v>
       </c>
-      <c r="C1" s="96"/>
-      <c r="D1" s="96"/>
-      <c r="E1" s="96"/>
+      <c r="C1" s="90"/>
+      <c r="D1" s="90"/>
+      <c r="E1" s="90"/>
     </row>
     <row r="2" spans="1:6" ht="36.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B2" s="46" t="s">
@@ -1604,10 +1606,10 @@
       </c>
     </row>
     <row r="3" spans="1:6" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="97" t="s">
+      <c r="B3" s="91" t="s">
         <v>61</v>
       </c>
-      <c r="C3" s="97"/>
+      <c r="C3" s="91"/>
       <c r="D3" s="47"/>
       <c r="E3" s="47"/>
       <c r="F3" s="45" t="s">
@@ -1619,28 +1621,28 @@
         <v>36</v>
       </c>
       <c r="C4" s="49"/>
-      <c r="D4" s="98" t="s">
+      <c r="D4" s="92" t="s">
         <v>35</v>
       </c>
-      <c r="E4" s="98"/>
+      <c r="E4" s="92"/>
     </row>
     <row r="5" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="99" t="s">
+      <c r="B5" s="93" t="s">
         <v>37</v>
       </c>
-      <c r="C5" s="99"/>
+      <c r="C5" s="93"/>
     </row>
     <row r="6" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="97" t="s">
+      <c r="B6" s="91" t="s">
         <v>38</v>
       </c>
-      <c r="C6" s="97"/>
+      <c r="C6" s="91"/>
     </row>
     <row r="7" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="97" t="s">
+      <c r="B7" s="91" t="s">
         <v>2</v>
       </c>
-      <c r="C7" s="97"/>
+      <c r="C7" s="91"/>
     </row>
     <row r="8" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="50"/>
@@ -1660,7 +1662,7 @@
       </c>
       <c r="C10" s="52"/>
     </row>
-    <row r="11" spans="1:6" s="54" customFormat="1" ht="11.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" ht="11.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="51"/>
       <c r="B11" s="52" t="s">
         <v>45</v>
@@ -1678,53 +1680,53 @@
     </row>
     <row r="13" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="51"/>
-      <c r="B13" s="57" t="s">
+      <c r="B13" s="55" t="s">
         <v>41</v>
       </c>
-      <c r="C13" s="57" t="s">
+      <c r="C13" s="55" t="s">
         <v>22</v>
       </c>
-      <c r="D13" s="58" t="s">
+      <c r="D13" s="56" t="s">
         <v>42</v>
       </c>
-      <c r="E13" s="57" t="s">
+      <c r="E13" s="55" t="s">
         <v>35</v>
       </c>
-      <c r="F13" s="59" t="s">
+      <c r="F13" s="57" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="84" t="s">
+      <c r="B14" s="82" t="s">
         <v>35</v>
       </c>
-      <c r="C14" s="55"/>
-      <c r="D14" s="85"/>
-      <c r="E14" s="56"/>
-      <c r="F14" s="86"/>
+      <c r="C14" s="48"/>
+      <c r="D14" s="83"/>
+      <c r="E14" s="54"/>
+      <c r="F14" s="84"/>
     </row>
     <row r="15" spans="1:6" ht="24" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="60" t="s">
+      <c r="B15" s="58" t="s">
         <v>44</v>
       </c>
-      <c r="C15" s="60"/>
-      <c r="D15" s="61"/>
-      <c r="E15" s="60"/>
-      <c r="F15" s="62"/>
+      <c r="C15" s="58"/>
+      <c r="D15" s="59"/>
+      <c r="E15" s="58"/>
+      <c r="F15" s="60"/>
     </row>
     <row r="16" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="95" t="s">
+      <c r="B16" s="89" t="s">
         <v>35</v>
       </c>
-      <c r="C16" s="95"/>
-      <c r="D16" s="95"/>
+      <c r="C16" s="89"/>
+      <c r="D16" s="89"/>
     </row>
     <row r="17" spans="2:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="95" t="s">
+      <c r="B17" s="89" t="s">
         <v>35</v>
       </c>
-      <c r="C17" s="95"/>
-      <c r="D17" s="95"/>
+      <c r="C17" s="89"/>
+      <c r="D17" s="89"/>
     </row>
   </sheetData>
   <mergeCells count="8">
@@ -1797,37 +1799,37 @@
   <sheetData>
     <row r="1" spans="1:27" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A1" s="1"/>
-      <c r="K1" s="105" t="s">
+      <c r="K1" s="99" t="s">
         <v>0</v>
       </c>
-      <c r="L1" s="106"/>
-      <c r="M1" s="106"/>
+      <c r="L1" s="100"/>
+      <c r="M1" s="100"/>
     </row>
     <row r="2" spans="1:27" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G2" s="3"/>
       <c r="I2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="K2" s="106"/>
-      <c r="L2" s="106"/>
-      <c r="M2" s="106"/>
+      <c r="K2" s="100"/>
+      <c r="L2" s="100"/>
+      <c r="M2" s="100"/>
     </row>
     <row r="3" spans="1:27" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G3" s="5"/>
       <c r="I3" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="K3" s="106"/>
-      <c r="L3" s="106"/>
-      <c r="M3" s="106"/>
+      <c r="K3" s="100"/>
+      <c r="L3" s="100"/>
+      <c r="M3" s="100"/>
     </row>
     <row r="4" spans="1:27" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I4" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="K4" s="106"/>
-      <c r="L4" s="106"/>
-      <c r="M4" s="106"/>
+      <c r="K4" s="100"/>
+      <c r="L4" s="100"/>
+      <c r="M4" s="100"/>
     </row>
     <row r="5" spans="1:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="6" spans="1:27" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -1837,18 +1839,18 @@
       <c r="B6" s="8"/>
       <c r="C6" s="8"/>
       <c r="D6" s="9"/>
-      <c r="E6" s="107" t="s">
+      <c r="E6" s="101" t="s">
         <v>5</v>
       </c>
-      <c r="F6" s="101"/>
-      <c r="G6" s="107" t="s">
+      <c r="F6" s="95"/>
+      <c r="G6" s="101" t="s">
         <v>6</v>
       </c>
-      <c r="H6" s="101"/>
-      <c r="I6" s="107" t="s">
+      <c r="H6" s="95"/>
+      <c r="I6" s="101" t="s">
         <v>7</v>
       </c>
-      <c r="J6" s="101"/>
+      <c r="J6" s="95"/>
       <c r="K6" s="10"/>
       <c r="L6" s="11" t="s">
         <v>8</v>
@@ -1876,18 +1878,18 @@
       <c r="B7" s="15"/>
       <c r="C7" s="15"/>
       <c r="D7" s="16"/>
-      <c r="E7" s="108" t="s">
+      <c r="E7" s="102" t="s">
         <v>10</v>
       </c>
-      <c r="F7" s="103"/>
-      <c r="G7" s="109" t="s">
+      <c r="F7" s="97"/>
+      <c r="G7" s="103" t="s">
         <v>11</v>
       </c>
-      <c r="H7" s="103"/>
-      <c r="I7" s="110">
+      <c r="H7" s="97"/>
+      <c r="I7" s="104">
         <v>43455</v>
       </c>
-      <c r="J7" s="103"/>
+      <c r="J7" s="97"/>
       <c r="K7" s="17"/>
       <c r="L7" s="18" t="s">
         <v>12</v>
@@ -1898,10 +1900,10 @@
       <c r="A8" s="20"/>
     </row>
     <row r="9" spans="1:27" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="100" t="s">
+      <c r="A9" s="94" t="s">
         <v>13</v>
       </c>
-      <c r="B9" s="101"/>
+      <c r="B9" s="95"/>
       <c r="C9" s="21"/>
       <c r="D9" s="22"/>
       <c r="E9" s="23" t="s">
@@ -1925,10 +1927,10 @@
       <c r="K9" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="L9" s="102" t="s">
+      <c r="L9" s="96" t="s">
         <v>21</v>
       </c>
-      <c r="M9" s="103"/>
+      <c r="M9" s="97"/>
     </row>
     <row r="10" spans="1:27" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="24" t="s">
@@ -1992,10 +1994,10 @@
       <c r="M11" s="32"/>
     </row>
     <row r="12" spans="1:27" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="104" t="s">
+      <c r="A12" s="98" t="s">
         <v>27</v>
       </c>
-      <c r="B12" s="103"/>
+      <c r="B12" s="97"/>
       <c r="C12" s="30"/>
       <c r="D12" s="33"/>
       <c r="E12" s="32">

</xml_diff>